<commit_message>
Atualização automática de RODEIO_BONITO.xlsx
</commit_message>
<xml_diff>
--- a/RODEIO_BONITO.xlsx
+++ b/RODEIO_BONITO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gera-fichas\Comarcas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B5B385A8-909C-4774-B08D-8084EF880E75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{EC8CE54B-F9C3-4F5B-A331-352BD43E95F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1135,7 +1135,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1" xr:uid="{2926D546-3D7C-4DBB-9E7E-98951D89C68B}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{5F1B56E1-2F30-47F1-B55F-F082B5B520D4}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1165,10 +1165,10 @@
         <xdr:cNvPr id="2" name="Chart1" title="Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{661577B1-2C53-43A2-9FCC-0833CCA54AA7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C92FCF31-BFE3-418F-89D2-E738A6CA894A}"/>
             </a:ext>
             <a:ext uri="GoogleSheetsCustomDataVersion1">
-              <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" pictureOfChart="1"/>
+              <go:sheetsCustomData xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:go="http://customooxmlschemas.google.com/" pictureOfChart="1"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1206,7 +1206,7 @@
         <xdr:cNvPr id="3" name="Shape 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{40D12FDB-5A6B-449A-A8A8-F94AF73DA061}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C40D2456-3FA2-4144-8570-B0D1DE551F69}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1269,7 +1269,7 @@
         <xdr:cNvPr id="4" name="Shape 2" title="Desenho">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{46493452-98C6-46DF-832E-CC93A202CB6C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5A0CDC30-2DBC-4EFA-BC5E-CFE15D08F2EB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1288,7 +1288,7 @@
           <xdr:cNvPr id="5" name="Shape 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A30AAD08-ABE6-F8C7-830A-70CD46A5C6D9}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{45FF6833-A249-AED1-C70C-FB93FE9951BE}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1337,7 +1337,7 @@
           <xdr:cNvPr id="6" name="Shape 5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{06D9BC50-9C0E-7226-2016-9A293C76E43F}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{585918F7-2A1F-A796-71B7-0EB73368C0E6}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1356,7 +1356,7 @@
             <xdr:cNvPr id="7" name="Shape 6">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7C2068DB-9089-63DB-04E5-ECAD0910456A}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{75DBB247-03C3-4FCB-3C18-44AF3C71739C}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1387,7 +1387,7 @@
             <xdr:cNvPr id="8" name="Shape 7">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3E5B6D81-44F6-9276-24D6-16ED14CE5A82}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5DA7A6BA-904A-3DCD-048F-7F0AC04FD3F6}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1418,7 +1418,7 @@
             <xdr:cNvPr id="9" name="Shape 8">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{13A9097A-725A-CECD-D9FF-83080678C944}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D71AA20D-C622-CE71-E7DE-F48DD0D38F40}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1461,7 +1461,7 @@
         <xdr:cNvPr id="10" name="image2.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4BF98FA9-7D2E-49BC-A383-5A3280CAD0DA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D7354DA7-DF27-458D-A6C4-C952EEE4F1E9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1499,7 +1499,7 @@
         <xdr:cNvPr id="11" name="image1.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5F18A890-BAE2-4F5E-896A-35B5B52DF9A7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{509DBCF2-51BC-4AD3-8051-D622F954EC4D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1542,7 +1542,7 @@
         <xdr:cNvPr id="12" name="Imagem 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8FA6BF0A-B1FD-45A1-924F-7A372837A369}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1FB3606C-54F1-4D95-9F01-48596DCE61A5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1855,7 +1855,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8E707CD-4202-42CC-B80F-7CD47538BFCF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{363877EF-E883-4D10-B2EE-4F6BA42A7B6B}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>

</xml_diff>